<commit_message>
improved some of the ordination graphs and re-ran and recoded bvstep analyses for warden
</commit_message>
<xml_diff>
--- a/raw_data/Esperance rainfall calculations to 2022.xlsx
+++ b/raw_data/Esperance rainfall calculations to 2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26223"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dpaw.sharepoint.com/teams/EcosystemScience/Wetland monitoring/Warden &amp; Gore waterbirds/Analysis/Warden-Gore 2022/Warden_2021/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dpaw.sharepoint.com/teams/EcosystemScience/Wetland monitoring/Warden &amp; Gore waterbirds/Analysis/Warden-Gore-2023/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{276545D1-F481-6941-A24E-3A948190289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAE28941-091A-426A-B9AC-164DE0BCF571}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="8_{276545D1-F481-6941-A24E-3A948190289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EE37279-4D54-4D4C-A283-A25DB34EED81}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Esperance stn 9789" sheetId="2" r:id="rId1"/>
@@ -3843,10 +3843,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$209</c:f>
+              <c:f>Sheet1!$E$2:$E$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="33">
                   <c:v>6083</c:v>
                 </c:pt>
@@ -3879,6 +3879,9 @@
                 </c:pt>
                 <c:pt idx="202">
                   <c:v>3807</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2068</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3945,9 +3948,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$209</c:f>
+              <c:f>Sheet1!$A$2:$A$230</c:f>
               <c:strCache>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>1-2004</c:v>
                 </c:pt>
@@ -4571,16 +4574,79 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>4-2021</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>5-2021</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6-2021</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>7-2021</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>8-2021</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>9-2021</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>10-2021</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>11-2021</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>12-2021</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1-2022</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2-2022</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3-2022</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4-2022</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>5-2022</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>6-2022</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>7-2022</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>8-2022</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>9-2022</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>10-2022</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>11-2022</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>12-2022</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1-2023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$209</c:f>
+              <c:f>Sheet1!$B$2:$B$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>18.914285714285718</c:v>
                 </c:pt>
@@ -5194,7 +5260,79 @@
                   <c:v>-268.59819387755152</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>-287.29819387755151</c:v>
+                  <c:v>-287.28390816326578</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>-294.8214081632658</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>-311.50508163265357</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>-304.60916326530662</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>-270.71324489795967</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>-258.33773469387802</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>-252.39773469387802</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>-260.71773469387801</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>-254.58973469387803</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>-207.86973469387803</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>-221.64573469387804</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>-240.71573469387803</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>-264.80144897959229</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>-278.73894897959229</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>-288.42262244898006</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>-272.92670408163315</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>-270.23078571428618</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>-268.05527551020458</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>-251.71527551020461</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>-197.23527551020459</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>-201.50727551020458</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>-138.58727551020456</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>-99.363275510204573</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>-105.83327551020457</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>-120.53327551020458</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5246,9 +5384,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$209</c:f>
+              <c:f>Sheet1!$A$2:$A$230</c:f>
               <c:strCache>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>1-2004</c:v>
                 </c:pt>
@@ -5872,16 +6010,79 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>4-2021</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>5-2021</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6-2021</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>7-2021</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>8-2021</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>9-2021</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>10-2021</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>11-2021</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>12-2021</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1-2022</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2-2022</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3-2022</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4-2022</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>5-2022</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>6-2022</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>7-2022</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>8-2022</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>9-2022</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>10-2022</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>11-2022</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>12-2022</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1-2023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$209</c:f>
+              <c:f>Sheet1!$C$2:$C$230</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>5.853191489361695</c:v>
                 </c:pt>
@@ -6496,6 +6697,78 @@
                 </c:pt>
                 <c:pt idx="204">
                   <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="205" formatCode="General">
+                  <c:v>9.0486961896752724</c:v>
+                </c:pt>
+                <c:pt idx="206" formatCode="General">
+                  <c:v>31.159565754892668</c:v>
+                </c:pt>
+                <c:pt idx="207" formatCode="General">
+                  <c:v>18.839785535112448</c:v>
+                </c:pt>
+                <c:pt idx="208" formatCode="General">
+                  <c:v>35.246378941705849</c:v>
+                </c:pt>
+                <c:pt idx="209" formatCode="General">
+                  <c:v>53.126378941705845</c:v>
+                </c:pt>
+                <c:pt idx="210" formatCode="General">
+                  <c:v>51.77526783059475</c:v>
+                </c:pt>
+                <c:pt idx="211" formatCode="General">
+                  <c:v>44.358413898010504</c:v>
+                </c:pt>
+                <c:pt idx="212" formatCode="General">
+                  <c:v>32.796344932493248</c:v>
+                </c:pt>
+                <c:pt idx="213" formatCode="General">
+                  <c:v>69.839526750675049</c:v>
+                </c:pt>
+                <c:pt idx="214" formatCode="General">
+                  <c:v>60.650890387038679</c:v>
+                </c:pt>
+                <c:pt idx="215" formatCode="General">
+                  <c:v>41.669281191636372</c:v>
+                </c:pt>
+                <c:pt idx="216" formatCode="General">
+                  <c:v>31.322472680998068</c:v>
+                </c:pt>
+                <c:pt idx="217" formatCode="General">
+                  <c:v>17.46921181143286</c:v>
+                </c:pt>
+                <c:pt idx="218" formatCode="General">
+                  <c:v>4.1800813766502536</c:v>
+                </c:pt>
+                <c:pt idx="219" formatCode="General">
+                  <c:v>43.260301156870028</c:v>
+                </c:pt>
+                <c:pt idx="220" formatCode="General">
+                  <c:v>26.366894563463426</c:v>
+                </c:pt>
+                <c:pt idx="221" formatCode="General">
+                  <c:v>12.446894563463424</c:v>
+                </c:pt>
+                <c:pt idx="222" formatCode="General">
+                  <c:v>16.395783452352326</c:v>
+                </c:pt>
+                <c:pt idx="223" formatCode="General">
+                  <c:v>69.378929519768064</c:v>
+                </c:pt>
+                <c:pt idx="224" formatCode="General">
+                  <c:v>40.616860554250806</c:v>
+                </c:pt>
+                <c:pt idx="225" formatCode="General">
+                  <c:v>103.96004237243261</c:v>
+                </c:pt>
+                <c:pt idx="226" formatCode="General">
+                  <c:v>149.47140600879624</c:v>
+                </c:pt>
+                <c:pt idx="227" formatCode="General">
+                  <c:v>142.78979681339393</c:v>
+                </c:pt>
+                <c:pt idx="228" formatCode="General">
+                  <c:v>128.68979681339394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6547,9 +6820,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$209</c:f>
+              <c:f>Sheet1!$A$2:$A$230</c:f>
               <c:strCache>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>1-2004</c:v>
                 </c:pt>
@@ -7173,16 +7446,79 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>4-2021</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>5-2021</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6-2021</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>7-2021</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>8-2021</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>9-2021</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>10-2021</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>11-2021</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>12-2021</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1-2022</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2-2022</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3-2022</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4-2022</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>5-2022</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>6-2022</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>7-2022</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>8-2022</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>9-2022</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>10-2022</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>11-2022</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>12-2022</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1-2023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$209</c:f>
+              <c:f>Sheet1!$D$2:$D$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>0.80000000000000071</c:v>
                 </c:pt>
@@ -7797,6 +8133,78 @@
                 </c:pt>
                 <c:pt idx="204">
                   <c:v>141.40000000000018</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>132.30000000000018</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>122.00000000000018</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>124.00000000000018</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>159.9000000000002</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>187.20000000000022</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>187.00000000000023</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>174.30000000000024</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>165.00000000000023</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>210.50000000000023</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>204.00000000000023</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>167.50000000000023</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>147.50000000000023</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>135.40000000000023</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>121.90000000000023</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>153.70000000000024</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>128.80000000000024</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>127.30000000000024</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>131.50000000000023</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>170.20000000000022</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>155.9000000000002</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>222.0000000000002</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>257.70000000000022</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>234.00000000000023</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>219.00000000000023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8319,10 +8727,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$209</c:f>
+              <c:f>Sheet1!$F$2:$F$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="49">
                   <c:v>15269</c:v>
                 </c:pt>
@@ -8349,13 +8757,16 @@
                 </c:pt>
                 <c:pt idx="205">
                   <c:v>11370</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>14997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A13C-BB45-BDD9-9A6014AF6F8E}"/>
+              <c16:uniqueId val="{00000000-B77F-49D6-A11B-2A5396681AF6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8415,9 +8826,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$209</c:f>
+              <c:f>Sheet1!$A$2:$A$230</c:f>
               <c:strCache>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>1-2004</c:v>
                 </c:pt>
@@ -9041,16 +9452,79 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>4-2021</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>5-2021</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6-2021</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>7-2021</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>8-2021</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>9-2021</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>10-2021</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>11-2021</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>12-2021</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1-2022</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2-2022</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3-2022</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4-2022</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>5-2022</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>6-2022</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>7-2022</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>8-2022</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>9-2022</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>10-2022</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>11-2022</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>12-2022</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1-2023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$209</c:f>
+              <c:f>Sheet1!$B$2:$B$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>18.914285714285718</c:v>
                 </c:pt>
@@ -9664,7 +10138,79 @@
                   <c:v>-268.59819387755152</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>-287.29819387755151</c:v>
+                  <c:v>-287.28390816326578</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>-294.8214081632658</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>-311.50508163265357</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>-304.60916326530662</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>-270.71324489795967</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>-258.33773469387802</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>-252.39773469387802</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>-260.71773469387801</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>-254.58973469387803</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>-207.86973469387803</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>-221.64573469387804</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>-240.71573469387803</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>-264.80144897959229</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>-278.73894897959229</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>-288.42262244898006</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>-272.92670408163315</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>-270.23078571428618</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>-268.05527551020458</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>-251.71527551020461</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>-197.23527551020459</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>-201.50727551020458</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>-138.58727551020456</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>-99.363275510204573</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>-105.83327551020457</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>-120.53327551020458</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9672,7 +10218,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A13C-BB45-BDD9-9A6014AF6F8E}"/>
+              <c16:uniqueId val="{00000001-B77F-49D6-A11B-2A5396681AF6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9716,9 +10262,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$209</c:f>
+              <c:f>Sheet1!$A$2:$A$230</c:f>
               <c:strCache>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>1-2004</c:v>
                 </c:pt>
@@ -10342,16 +10888,79 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>4-2021</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>5-2021</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6-2021</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>7-2021</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>8-2021</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>9-2021</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>10-2021</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>11-2021</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>12-2021</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1-2022</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2-2022</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3-2022</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4-2022</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>5-2022</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>6-2022</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>7-2022</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>8-2022</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>9-2022</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>10-2022</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>11-2022</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>12-2022</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1-2023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$209</c:f>
+              <c:f>Sheet1!$C$2:$C$230</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>5.853191489361695</c:v>
                 </c:pt>
@@ -10966,6 +11575,78 @@
                 </c:pt>
                 <c:pt idx="204">
                   <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="205" formatCode="General">
+                  <c:v>9.0486961896752724</c:v>
+                </c:pt>
+                <c:pt idx="206" formatCode="General">
+                  <c:v>31.159565754892668</c:v>
+                </c:pt>
+                <c:pt idx="207" formatCode="General">
+                  <c:v>18.839785535112448</c:v>
+                </c:pt>
+                <c:pt idx="208" formatCode="General">
+                  <c:v>35.246378941705849</c:v>
+                </c:pt>
+                <c:pt idx="209" formatCode="General">
+                  <c:v>53.126378941705845</c:v>
+                </c:pt>
+                <c:pt idx="210" formatCode="General">
+                  <c:v>51.77526783059475</c:v>
+                </c:pt>
+                <c:pt idx="211" formatCode="General">
+                  <c:v>44.358413898010504</c:v>
+                </c:pt>
+                <c:pt idx="212" formatCode="General">
+                  <c:v>32.796344932493248</c:v>
+                </c:pt>
+                <c:pt idx="213" formatCode="General">
+                  <c:v>69.839526750675049</c:v>
+                </c:pt>
+                <c:pt idx="214" formatCode="General">
+                  <c:v>60.650890387038679</c:v>
+                </c:pt>
+                <c:pt idx="215" formatCode="General">
+                  <c:v>41.669281191636372</c:v>
+                </c:pt>
+                <c:pt idx="216" formatCode="General">
+                  <c:v>31.322472680998068</c:v>
+                </c:pt>
+                <c:pt idx="217" formatCode="General">
+                  <c:v>17.46921181143286</c:v>
+                </c:pt>
+                <c:pt idx="218" formatCode="General">
+                  <c:v>4.1800813766502536</c:v>
+                </c:pt>
+                <c:pt idx="219" formatCode="General">
+                  <c:v>43.260301156870028</c:v>
+                </c:pt>
+                <c:pt idx="220" formatCode="General">
+                  <c:v>26.366894563463426</c:v>
+                </c:pt>
+                <c:pt idx="221" formatCode="General">
+                  <c:v>12.446894563463424</c:v>
+                </c:pt>
+                <c:pt idx="222" formatCode="General">
+                  <c:v>16.395783452352326</c:v>
+                </c:pt>
+                <c:pt idx="223" formatCode="General">
+                  <c:v>69.378929519768064</c:v>
+                </c:pt>
+                <c:pt idx="224" formatCode="General">
+                  <c:v>40.616860554250806</c:v>
+                </c:pt>
+                <c:pt idx="225" formatCode="General">
+                  <c:v>103.96004237243261</c:v>
+                </c:pt>
+                <c:pt idx="226" formatCode="General">
+                  <c:v>149.47140600879624</c:v>
+                </c:pt>
+                <c:pt idx="227" formatCode="General">
+                  <c:v>142.78979681339393</c:v>
+                </c:pt>
+                <c:pt idx="228" formatCode="General">
+                  <c:v>128.68979681339394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10973,7 +11654,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A13C-BB45-BDD9-9A6014AF6F8E}"/>
+              <c16:uniqueId val="{00000002-B77F-49D6-A11B-2A5396681AF6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11017,9 +11698,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$209</c:f>
+              <c:f>Sheet1!$A$2:$A$230</c:f>
               <c:strCache>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>1-2004</c:v>
                 </c:pt>
@@ -11643,16 +12324,79 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>4-2021</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>5-2021</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6-2021</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>7-2021</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>8-2021</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>9-2021</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>10-2021</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>11-2021</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>12-2021</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1-2022</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2-2022</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3-2022</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4-2022</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>5-2022</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>6-2022</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>7-2022</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>8-2022</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>9-2022</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>10-2022</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>11-2022</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>12-2022</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1-2023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$209</c:f>
+              <c:f>Sheet1!$D$2:$D$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="208"/>
+                <c:ptCount val="229"/>
                 <c:pt idx="0">
                   <c:v>0.80000000000000071</c:v>
                 </c:pt>
@@ -12267,6 +13011,78 @@
                 </c:pt>
                 <c:pt idx="204">
                   <c:v>141.40000000000018</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>132.30000000000018</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>122.00000000000018</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>124.00000000000018</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>159.9000000000002</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>187.20000000000022</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>187.00000000000023</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>174.30000000000024</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>165.00000000000023</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>210.50000000000023</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>204.00000000000023</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>167.50000000000023</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>147.50000000000023</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>135.40000000000023</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>121.90000000000023</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>153.70000000000024</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>128.80000000000024</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>127.30000000000024</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>131.50000000000023</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>170.20000000000022</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>155.9000000000002</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>222.0000000000002</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>257.70000000000022</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>234.00000000000023</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>219.00000000000023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12274,7 +13090,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-A13C-BB45-BDD9-9A6014AF6F8E}"/>
+              <c16:uniqueId val="{00000003-B77F-49D6-A11B-2A5396681AF6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12518,6 +13334,7 @@
         <c:axId val="1198797599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="30000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -16058,13 +16875,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1193800</xdr:colOff>
+      <xdr:colOff>755650</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>60324</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>269875</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
@@ -16093,23 +16910,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>206375</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF96ED6E-1648-4942-A125-3988A60BA81A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4A8DFE3-8206-4DEE-9A00-9AAB16108474}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{930C511F-4B47-4908-84E4-47F886A4E291}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16473,8 +17293,8 @@
   <dimension ref="A1:Y231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F204" sqref="F204"/>
+      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J228" sqref="J228:J230"/>
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -24278,7 +25098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF79CE5-BBE4-4252-87B4-EC41CE376203}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
@@ -24293,7 +25113,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -24487,8 +25307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42734D63-6FA6-4A85-92AC-8ED2F50789B0}">
   <dimension ref="A1:O231"/>
   <sheetViews>
-    <sheetView topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="E218" sqref="E218"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="J227" sqref="J227:J230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -31107,21 +31927,19 @@
         <v>10</v>
       </c>
       <c r="E227">
-        <v>106</v>
-      </c>
-      <c r="F227" s="4">
-        <v>106</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="F227" s="15"/>
       <c r="H227" s="5">
         <v>52.656818181818196</v>
       </c>
       <c r="I227" s="5">
         <f t="shared" si="8"/>
-        <v>53.343181818181804</v>
+        <v>63.343181818181804</v>
       </c>
       <c r="J227" s="5">
         <f t="shared" si="9"/>
-        <v>93.960042372432611</v>
+        <v>103.96004237243261</v>
       </c>
     </row>
     <row r="228" spans="1:13">
@@ -31149,19 +31967,19 @@
       </c>
       <c r="J228" s="5">
         <f t="shared" si="9"/>
-        <v>139.47140600879624</v>
+        <v>149.47140600879624</v>
       </c>
       <c r="K228" s="1">
         <f>SUM(I225:I227)</f>
-        <v>77.564258920080292</v>
+        <v>87.564258920080292</v>
       </c>
       <c r="L228" s="1">
         <f>SUM(I222:I227)</f>
-        <v>50.69974121556259</v>
+        <v>60.69974121556259</v>
       </c>
       <c r="M228" s="1">
         <f>SUM(I216:I227)</f>
-        <v>24.120515621757569</v>
+        <v>34.120515621757569</v>
       </c>
     </row>
     <row r="229" spans="1:13">
@@ -31189,7 +32007,7 @@
       </c>
       <c r="J229" s="5">
         <f t="shared" si="9"/>
-        <v>132.78979681339393</v>
+        <v>142.78979681339393</v>
       </c>
     </row>
     <row r="230" spans="1:13">
@@ -31207,6 +32025,17 @@
       </c>
       <c r="E230" s="15">
         <v>8.9</v>
+      </c>
+      <c r="H230" s="5">
+        <v>23</v>
+      </c>
+      <c r="I230" s="5">
+        <f t="shared" ref="I230" si="10">E230-H230</f>
+        <v>-14.1</v>
+      </c>
+      <c r="J230" s="5">
+        <f t="shared" ref="J230" si="11">J229+I230</f>
+        <v>128.68979681339394</v>
       </c>
     </row>
     <row r="231" spans="1:13">
@@ -31218,15 +32047,15 @@
       </c>
       <c r="K231" s="1">
         <f>SUM(I228:I230)</f>
-        <v>38.829754440961324</v>
+        <v>24.729754440961322</v>
       </c>
       <c r="L231" s="1">
         <f>SUM(I225:I230)</f>
-        <v>116.39401336104163</v>
+        <v>112.29401336104164</v>
       </c>
       <c r="M231" s="1">
         <f>SUM(I219:I230)</f>
-        <v>101.46732413239587</v>
+        <v>97.367324132395879</v>
       </c>
     </row>
   </sheetData>
@@ -31238,8 +32067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAC6E81-9653-403C-AD85-0661500D04DB}">
   <dimension ref="A1:O231"/>
   <sheetViews>
-    <sheetView topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="K207" sqref="K207:M207"/>
+    <sheetView topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="G233" sqref="G233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -38002,7 +38831,7 @@
   <dimension ref="A1:G191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -41266,10 +42095,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAC69FA-8365-4B6A-924D-E0BC820D6526}">
-  <dimension ref="A1:F225"/>
+  <dimension ref="A1:I241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D204" sqref="D204"/>
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D228" sqref="D228:D230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -44220,7 +45050,7 @@
         <v>44197</v>
       </c>
       <c r="B206">
-        <v>-287.29819387755151</v>
+        <v>-287.28390816326578</v>
       </c>
       <c r="C206" s="5">
         <v>2.2999999999999998</v>
@@ -44233,6 +45063,15 @@
       <c r="A207" s="14">
         <v>44228</v>
       </c>
+      <c r="B207">
+        <v>-294.8214081632658</v>
+      </c>
+      <c r="C207">
+        <v>9.0486961896752724</v>
+      </c>
+      <c r="D207">
+        <v>132.30000000000018</v>
+      </c>
       <c r="F207">
         <v>11370</v>
       </c>
@@ -44241,59 +45080,386 @@
       <c r="A208" s="14">
         <v>44256</v>
       </c>
-    </row>
-    <row r="209" spans="1:1">
+      <c r="B208">
+        <v>-311.50508163265357</v>
+      </c>
+      <c r="C208">
+        <v>31.159565754892668</v>
+      </c>
+      <c r="D208">
+        <v>122.00000000000018</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
       <c r="A209" s="14">
         <v>44287</v>
       </c>
-    </row>
-    <row r="210" spans="1:1">
-      <c r="A210" s="14"/>
-    </row>
-    <row r="211" spans="1:1">
-      <c r="A211" s="14"/>
-    </row>
-    <row r="212" spans="1:1">
-      <c r="A212" s="14"/>
-    </row>
-    <row r="213" spans="1:1">
-      <c r="A213" s="14"/>
-    </row>
-    <row r="214" spans="1:1">
-      <c r="A214" s="14"/>
-    </row>
-    <row r="215" spans="1:1">
-      <c r="A215" s="14"/>
-    </row>
-    <row r="216" spans="1:1">
-      <c r="A216" s="14"/>
-    </row>
-    <row r="217" spans="1:1">
-      <c r="A217" s="14"/>
-    </row>
-    <row r="218" spans="1:1">
-      <c r="A218" s="14"/>
-    </row>
-    <row r="219" spans="1:1">
-      <c r="A219" s="14"/>
-    </row>
-    <row r="220" spans="1:1">
-      <c r="A220" s="14"/>
-    </row>
-    <row r="221" spans="1:1">
-      <c r="A221" s="14"/>
-    </row>
-    <row r="222" spans="1:1">
-      <c r="A222" s="14"/>
-    </row>
-    <row r="223" spans="1:1">
-      <c r="A223" s="14"/>
-    </row>
-    <row r="224" spans="1:1">
-      <c r="A224" s="14"/>
-    </row>
-    <row r="225" spans="1:1">
-      <c r="A225" s="14"/>
+      <c r="B209">
+        <v>-304.60916326530662</v>
+      </c>
+      <c r="C209">
+        <v>18.839785535112448</v>
+      </c>
+      <c r="D209">
+        <v>124.00000000000018</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" s="14">
+        <v>44317</v>
+      </c>
+      <c r="B210">
+        <v>-270.71324489795967</v>
+      </c>
+      <c r="C210">
+        <v>35.246378941705849</v>
+      </c>
+      <c r="D210">
+        <v>159.9000000000002</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" s="14">
+        <v>44348</v>
+      </c>
+      <c r="B211">
+        <v>-258.33773469387802</v>
+      </c>
+      <c r="C211">
+        <v>53.126378941705845</v>
+      </c>
+      <c r="D211">
+        <v>187.20000000000022</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="14">
+        <v>44378</v>
+      </c>
+      <c r="B212">
+        <v>-252.39773469387802</v>
+      </c>
+      <c r="C212">
+        <v>51.77526783059475</v>
+      </c>
+      <c r="D212">
+        <v>187.00000000000023</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="14">
+        <v>44409</v>
+      </c>
+      <c r="B213">
+        <v>-260.71773469387801</v>
+      </c>
+      <c r="C213">
+        <v>44.358413898010504</v>
+      </c>
+      <c r="D213">
+        <v>174.30000000000024</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" s="14">
+        <v>44440</v>
+      </c>
+      <c r="B214">
+        <v>-254.58973469387803</v>
+      </c>
+      <c r="C214">
+        <v>32.796344932493248</v>
+      </c>
+      <c r="D214">
+        <v>165.00000000000023</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" s="14">
+        <v>44470</v>
+      </c>
+      <c r="B215">
+        <v>-207.86973469387803</v>
+      </c>
+      <c r="C215">
+        <v>69.839526750675049</v>
+      </c>
+      <c r="D215">
+        <v>210.50000000000023</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" s="14">
+        <v>44501</v>
+      </c>
+      <c r="B216">
+        <v>-221.64573469387804</v>
+      </c>
+      <c r="C216">
+        <v>60.650890387038679</v>
+      </c>
+      <c r="D216">
+        <v>204.00000000000023</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" s="14">
+        <v>44531</v>
+      </c>
+      <c r="B217">
+        <v>-240.71573469387803</v>
+      </c>
+      <c r="C217">
+        <v>41.669281191636372</v>
+      </c>
+      <c r="D217">
+        <v>167.50000000000023</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" s="14">
+        <v>44562</v>
+      </c>
+      <c r="B218">
+        <v>-264.80144897959229</v>
+      </c>
+      <c r="C218">
+        <v>31.322472680998068</v>
+      </c>
+      <c r="D218">
+        <v>147.50000000000023</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" s="14">
+        <v>44593</v>
+      </c>
+      <c r="B219">
+        <v>-278.73894897959229</v>
+      </c>
+      <c r="C219">
+        <v>17.46921181143286</v>
+      </c>
+      <c r="D219">
+        <v>135.40000000000023</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" s="14">
+        <v>44621</v>
+      </c>
+      <c r="B220">
+        <v>-288.42262244898006</v>
+      </c>
+      <c r="C220">
+        <v>4.1800813766502536</v>
+      </c>
+      <c r="D220">
+        <v>121.90000000000023</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="14">
+        <v>44652</v>
+      </c>
+      <c r="B221">
+        <v>-272.92670408163315</v>
+      </c>
+      <c r="C221">
+        <v>43.260301156870028</v>
+      </c>
+      <c r="D221">
+        <v>153.70000000000024</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="14">
+        <v>44682</v>
+      </c>
+      <c r="B222">
+        <v>-270.23078571428618</v>
+      </c>
+      <c r="C222">
+        <v>26.366894563463426</v>
+      </c>
+      <c r="D222">
+        <v>128.80000000000024</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" s="14">
+        <v>44713</v>
+      </c>
+      <c r="B223">
+        <v>-268.05527551020458</v>
+      </c>
+      <c r="C223">
+        <v>12.446894563463424</v>
+      </c>
+      <c r="D223">
+        <v>127.30000000000024</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" s="14">
+        <v>44743</v>
+      </c>
+      <c r="B224">
+        <v>-251.71527551020461</v>
+      </c>
+      <c r="C224">
+        <v>16.395783452352326</v>
+      </c>
+      <c r="D224">
+        <v>131.50000000000023</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9">
+      <c r="A225" s="14">
+        <v>44774</v>
+      </c>
+      <c r="B225">
+        <v>-197.23527551020459</v>
+      </c>
+      <c r="C225">
+        <v>69.378929519768064</v>
+      </c>
+      <c r="D225">
+        <v>170.20000000000022</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9">
+      <c r="A226" s="14">
+        <v>44805</v>
+      </c>
+      <c r="B226">
+        <v>-201.50727551020458</v>
+      </c>
+      <c r="C226">
+        <v>40.616860554250806</v>
+      </c>
+      <c r="D226">
+        <v>155.9000000000002</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9">
+      <c r="A227" s="14">
+        <v>44835</v>
+      </c>
+      <c r="B227">
+        <v>-138.58727551020456</v>
+      </c>
+      <c r="C227">
+        <v>103.96004237243261</v>
+      </c>
+      <c r="D227">
+        <v>222.0000000000002</v>
+      </c>
+      <c r="I227">
+        <v>103.96004237243261</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9">
+      <c r="A228" s="14">
+        <v>44866</v>
+      </c>
+      <c r="B228">
+        <v>-99.363275510204573</v>
+      </c>
+      <c r="C228">
+        <v>149.47140600879624</v>
+      </c>
+      <c r="D228">
+        <v>257.70000000000022</v>
+      </c>
+      <c r="E228">
+        <v>2068</v>
+      </c>
+      <c r="I228">
+        <v>149.47140600879624</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9">
+      <c r="A229" s="14">
+        <v>44896</v>
+      </c>
+      <c r="B229">
+        <v>-105.83327551020457</v>
+      </c>
+      <c r="C229">
+        <v>142.78979681339393</v>
+      </c>
+      <c r="D229">
+        <v>234.00000000000023</v>
+      </c>
+      <c r="I229">
+        <v>142.78979681339393</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9">
+      <c r="A230" s="14">
+        <v>44927</v>
+      </c>
+      <c r="B230">
+        <v>-120.53327551020458</v>
+      </c>
+      <c r="C230">
+        <v>128.68979681339394</v>
+      </c>
+      <c r="D230">
+        <v>219.00000000000023</v>
+      </c>
+      <c r="F230">
+        <v>14997</v>
+      </c>
+      <c r="I230">
+        <v>128.68979681339394</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9">
+      <c r="A231"/>
+    </row>
+    <row r="232" spans="1:9">
+      <c r="A232"/>
+      <c r="B232">
+        <f>B227-B204</f>
+        <v>117.34091836734694</v>
+      </c>
+      <c r="C232">
+        <f>C227-C204</f>
+        <v>73.729667607151526</v>
+      </c>
+      <c r="D232">
+        <f t="shared" ref="D232" si="0">D227-D204</f>
+        <v>35.30000000000004</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9">
+      <c r="A233"/>
+    </row>
+    <row r="234" spans="1:9">
+      <c r="A234"/>
+    </row>
+    <row r="235" spans="1:9">
+      <c r="A235"/>
+    </row>
+    <row r="236" spans="1:9">
+      <c r="A236"/>
+    </row>
+    <row r="237" spans="1:9">
+      <c r="A237"/>
+    </row>
+    <row r="238" spans="1:9">
+      <c r="A238"/>
+    </row>
+    <row r="239" spans="1:9">
+      <c r="A239"/>
+    </row>
+    <row r="240" spans="1:9">
+      <c r="A240"/>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>